<commit_message>
cambios en prueba_web ya puede insertar los datos en el excel
</commit_message>
<xml_diff>
--- a/RPA-EOI/excel/Libro1.xlsx
+++ b/RPA-EOI/excel/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\OneDrive\Documentos\REPO\RPA\EOI-RPA-Project\RPA-EOI\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AB8586-015C-45BD-96DE-CA3F31580159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D44D4-DC99-46A8-ADB8-FDC65A1C19F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4EBEB8D5-403A-42AB-88A7-34EF4201B689}"/>
   </bookViews>
@@ -36,12 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Nueva columna 0</t>
+    <t>Ingrediente</t>
   </si>
   <si>
-    <t>unchecked</t>
+    <t>500 gramos de hongos frescos                                                                                                        
+1½ litros de agua o fondo de verduras                                                                                                        
+1 pieza de cebolla mediana picada                                                                                                        
+2 dientes de ajo picados                                                                                                        
+2 cucharadas soperas de crema ácida                                                                                                        
+2 cucharadas soperas de mantequilla o margarina                                                                                                        
+sal y pimienta al gusto
+3 hojas de epazote picado                                                                                                        
+1 pizca de tomillo                                                                                                        
+2 hojas de laurel</t>
+  </si>
+  <si>
+    <t>4 comensales
+30m
+Entrante
+Dificultad baja</t>
   </si>
 </sst>
 </file>
@@ -416,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBAAED46-F28C-4F1E-B042-7BC0EABD02F4}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:A13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,55 +448,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
+    <row r="4" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
puesto la opcion de seguir
</commit_message>
<xml_diff>
--- a/RPA-EOI/excel/Libro1.xlsx
+++ b/RPA-EOI/excel/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\OneDrive\Documentos\REPO\RPA\EOI-RPA-Project\RPA-EOI\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5D44D4-DC99-46A8-ADB8-FDC65A1C19F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A4E7FE-E6A8-46DF-BD4E-DB2A6C84A050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4EBEB8D5-403A-42AB-88A7-34EF4201B689}"/>
   </bookViews>
@@ -41,21 +41,21 @@
     <t>Ingrediente</t>
   </si>
   <si>
-    <t>500 gramos de hongos frescos                                                                                                        
-1½ litros de agua o fondo de verduras                                                                                                        
-1 pieza de cebolla mediana picada                                                                                                        
-2 dientes de ajo picados                                                                                                        
-2 cucharadas soperas de crema ácida                                                                                                        
-2 cucharadas soperas de mantequilla o margarina                                                                                                        
-sal y pimienta al gusto
-3 hojas de epazote picado                                                                                                        
-1 pizca de tomillo                                                                                                        
-2 hojas de laurel</t>
+    <t>4 piezas de pollo                                                                                                        
+5 cucharadas soperas de ají panca en pasta                                                                                                        
+3 cucharadas soperas de ajo molido                                                                                                        
+1 cucharadita de comino molido                                                                                                        
+1 cucharadita de pimienta negra molida                                                                                                        
+1 cucharadita de orégano seco molido                                                                                                        
+2 cucharadas soperas de mostaza                                                                                                        
+100 mililitros de vinagre tinto                                                                                                        
+100 mililitros de sillao                                                                                                        
+3 cucharaditas de sal                                                                                                        
+aceite c/n</t>
   </si>
   <si>
     <t>4 comensales
-30m
-Entrante
+45m
 Dificultad baja</t>
   </si>
 </sst>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBAAED46-F28C-4F1E-B042-7BC0EABD02F4}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Corregido excel celdas vacias
</commit_message>
<xml_diff>
--- a/RPA-EOI/excel/Libro1.xlsx
+++ b/RPA-EOI/excel/Libro1.xlsx
@@ -406,7 +406,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B10"/>
+  <x:dimension ref="A1:B9"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -484,14 +484,6 @@
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:2">
-      <x:c r="A10" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>